<commit_message>
reduce oblect_id width for HEADER_ID uniqueness
</commit_message>
<xml_diff>
--- a/proto_ip_code/dataframe_generator/dataframe_format.xlsx
+++ b/proto_ip_code/dataframe_generator/dataframe_format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\npart\KRD\proto_ip_code\dataframe_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KRD\proto_ip_code\dataframe_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45467FA6-5FEB-41E8-8FBE-A6EA5AF7BFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D13C7E7-F336-4CE8-8138-0E042DED167B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47A0C5A6-AF27-41FE-9D29-76E50A9C23F1}"/>
   </bookViews>
@@ -243,10 +243,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>OBJECT_ID[31:24]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>OBJECT_ID[23:0]</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -255,7 +251,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Last Update: 2020/06/09</t>
+    <t>ZERO_PADING[7:0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Last Update: 2020/07/01</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -288,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -593,6 +593,26 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -601,7 +621,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -638,25 +658,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -665,52 +703,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1030,7 +1056,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1167,60 +1193,60 @@
       <c r="B4">
         <v>63</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="14" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="28"/>
       <c r="K4" s="11" t="s">
         <v>47</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="36"/>
+      <c r="M4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="17"/>
       <c r="S4" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="25" t="s">
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
       <c r="R5" s="35"/>
       <c r="S5" s="3"/>
     </row>
@@ -1228,123 +1254,123 @@
       <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
       <c r="K6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="22"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="13"/>
       <c r="O6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="P6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="32"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="14"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="26"/>
       <c r="K7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="19"/>
-      <c r="N7" s="20"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="26"/>
       <c r="O7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="P7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="31"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="27"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="24"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="32"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="37"/>
       <c r="K9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="20"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="26"/>
       <c r="O9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="P9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="31"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="27"/>
     </row>
     <row r="10" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -1353,30 +1379,30 @@
       <c r="B10">
         <v>63</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="13" t="s">
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="34"/>
-      <c r="K10" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="29" t="s">
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="R10" s="30"/>
+      <c r="R10" s="24"/>
       <c r="S10" s="3">
         <v>0</v>
       </c>
@@ -1514,11 +1540,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C8:R8"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H6:J6"/>
     <mergeCell ref="L6:N6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="M4:R4"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:J10"/>
     <mergeCell ref="K10:P10"/>
     <mergeCell ref="Q10:R10"/>
     <mergeCell ref="L9:N9"/>
@@ -1530,14 +1564,6 @@
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="H9:J9"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="C8:R8"/>
-    <mergeCell ref="K5:R5"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
move FOOTER_ID to top of footer
</commit_message>
<xml_diff>
--- a/proto_ip_code/dataframe_generator/dataframe_format.xlsx
+++ b/proto_ip_code/dataframe_generator/dataframe_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KRD\proto_ip_code\dataframe_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F73E55C-859A-433D-BD85-D996B91664BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EB2470-E39D-4B47-8969-9F71B3FBA595}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47A0C5A6-AF27-41FE-9D29-76E50A9C23F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
   <si>
     <t>HEADER</t>
     <phoneticPr fontId="1"/>
@@ -235,27 +235,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>OBJECT_ID[23:0]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>TIME_STAMP[23:0]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ZERO_PADING[7:0]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Last Update: 2020/07/13</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRAME_INFO [3:0] = {1'b0, TRIGGER_STATE[1:0],  FRAME_CONTINUE[0:0]}</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>* GAIN_TYPE is removed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Last Update: 2020/07/15</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OBJECT_ID[31:0]</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -288,7 +284,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -554,10 +550,10 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -565,18 +561,29 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -587,32 +594,12 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -655,7 +642,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -694,50 +705,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1056,7 +1043,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="K10" sqref="K10:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1193,184 +1180,184 @@
       <c r="B4">
         <v>63</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="27"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="11" t="s">
         <v>47</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="31"/>
+      <c r="M4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="19"/>
       <c r="S4" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="38"/>
+      <c r="E5" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="15" t="s">
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="17"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="25"/>
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="24"/>
-      <c r="J6" s="25"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
       <c r="K6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="24"/>
-      <c r="N6" s="25"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="17"/>
       <c r="O6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="30"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="18"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
       <c r="G7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="31"/>
       <c r="K7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="22"/>
-      <c r="N7" s="23"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="31"/>
       <c r="O7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="36"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="33"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="14"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="22"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
       <c r="K9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="22"/>
-      <c r="N9" s="23"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="31"/>
       <c r="O9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P9" s="22" t="s">
+      <c r="P9" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="36"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="33"/>
     </row>
     <row r="10" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -1379,30 +1366,28 @@
       <c r="B10">
         <v>63</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20" t="s">
+      <c r="C10" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="32" t="s">
-        <v>52</v>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="36" t="s">
+        <v>56</v>
       </c>
       <c r="L10" s="32"/>
       <c r="M10" s="32"/>
       <c r="N10" s="32"/>
       <c r="O10" s="32"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="R10" s="35"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="37"/>
       <c r="S10" s="3">
         <v>0</v>
       </c>
@@ -1515,7 +1500,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.4">
@@ -1530,7 +1515,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
@@ -1539,7 +1524,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="23">
+    <mergeCell ref="C8:R8"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K10:R10"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="H6:J6"/>
@@ -1549,21 +1548,6 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:J5"/>
-    <mergeCell ref="C8:R8"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="K10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="H9:J9"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>